<commit_message>
fix up columns and column aliaes
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/data-contracts/EOHHS-075-06302020-bad_proj_id-v1.xlsx
+++ b/tests/server/fixtures/data-contracts/EOHHS-075-06302020-bad_proj_id-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnmclaughlin/git/usdr/cares-reporter/tests/server/fixtures/data-contracts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14472A3-1804-2C42-B6B7-81ED170CFD34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7360294A-7869-8B4B-ADCD-CAD1DBD34988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="-18420" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1940" yWindow="-18420" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="340">
   <si>
     <t>Agency Code</t>
   </si>
@@ -1064,6 +1064,9 @@
   <si>
     <t>ID + Duns</t>
   </si>
+  <si>
+    <t>Sum of expenses</t>
+  </si>
 </sst>
 </file>
 
@@ -1073,7 +1076,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1136,6 +1139,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1287,7 +1296,7 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1378,6 +1387,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -11166,7 +11176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:K13"/>
     </sheetView>
   </sheetViews>
@@ -12153,8 +12163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AY984"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AP1" sqref="AP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12307,7 +12317,9 @@
       <c r="AO1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="AP1" s="4"/>
+      <c r="AP1" s="62" t="s">
+        <v>339</v>
+      </c>
       <c r="AQ1" s="4"/>
       <c r="AR1" s="4"/>
       <c r="AS1" s="4"/>
@@ -19575,10 +19587,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AQ998"/>
+  <dimension ref="A1:AR998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AR1" sqref="AR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -19600,7 +19612,7 @@
     <col min="33" max="43" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:44" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -19730,8 +19742,11 @@
       <c r="AQ1" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AR1" s="62" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="41" t="s">
         <v>239</v>
       </c>
@@ -19810,7 +19825,7 @@
       <c r="AP2" s="5"/>
       <c r="AQ2" s="5"/>
     </row>
-    <row r="3" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
@@ -19831,7 +19846,7 @@
       <c r="AP3" s="5"/>
       <c r="AQ3" s="5"/>
     </row>
-    <row r="4" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z4" s="5"/>
       <c r="AB4" s="5"/>
       <c r="AD4" s="5"/>
@@ -19848,7 +19863,7 @@
       <c r="AP4" s="5"/>
       <c r="AQ4" s="5"/>
     </row>
-    <row r="5" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z5" s="5"/>
       <c r="AB5" s="5"/>
       <c r="AD5" s="5"/>
@@ -19865,7 +19880,7 @@
       <c r="AP5" s="5"/>
       <c r="AQ5" s="5"/>
     </row>
-    <row r="6" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z6" s="5"/>
       <c r="AB6" s="5"/>
       <c r="AD6" s="5"/>
@@ -19882,7 +19897,7 @@
       <c r="AP6" s="5"/>
       <c r="AQ6" s="5"/>
     </row>
-    <row r="7" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z7" s="5"/>
       <c r="AB7" s="5"/>
       <c r="AD7" s="5"/>
@@ -19899,7 +19914,7 @@
       <c r="AP7" s="5"/>
       <c r="AQ7" s="5"/>
     </row>
-    <row r="8" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z8" s="5"/>
       <c r="AB8" s="5"/>
       <c r="AD8" s="5"/>
@@ -19916,7 +19931,7 @@
       <c r="AP8" s="5"/>
       <c r="AQ8" s="5"/>
     </row>
-    <row r="9" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z9" s="5"/>
       <c r="AB9" s="5"/>
       <c r="AD9" s="5"/>
@@ -19933,7 +19948,7 @@
       <c r="AP9" s="5"/>
       <c r="AQ9" s="5"/>
     </row>
-    <row r="10" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z10" s="5"/>
       <c r="AB10" s="5"/>
       <c r="AD10" s="5"/>
@@ -19950,7 +19965,7 @@
       <c r="AP10" s="5"/>
       <c r="AQ10" s="5"/>
     </row>
-    <row r="11" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z11" s="5"/>
       <c r="AB11" s="5"/>
       <c r="AD11" s="5"/>
@@ -19967,7 +19982,7 @@
       <c r="AP11" s="5"/>
       <c r="AQ11" s="5"/>
     </row>
-    <row r="12" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z12" s="5"/>
       <c r="AB12" s="5"/>
       <c r="AD12" s="5"/>
@@ -19984,7 +19999,7 @@
       <c r="AP12" s="5"/>
       <c r="AQ12" s="5"/>
     </row>
-    <row r="13" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z13" s="5"/>
       <c r="AB13" s="5"/>
       <c r="AD13" s="5"/>
@@ -20001,7 +20016,7 @@
       <c r="AP13" s="5"/>
       <c r="AQ13" s="5"/>
     </row>
-    <row r="14" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z14" s="5"/>
       <c r="AB14" s="5"/>
       <c r="AD14" s="5"/>
@@ -20018,7 +20033,7 @@
       <c r="AP14" s="5"/>
       <c r="AQ14" s="5"/>
     </row>
-    <row r="15" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z15" s="5"/>
       <c r="AB15" s="5"/>
       <c r="AD15" s="5"/>
@@ -20035,7 +20050,7 @@
       <c r="AP15" s="5"/>
       <c r="AQ15" s="5"/>
     </row>
-    <row r="16" spans="1:43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="Z16" s="5"/>
       <c r="AB16" s="5"/>
       <c r="AD16" s="5"/>
@@ -36758,10 +36773,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AM1000"/>
+  <dimension ref="A1:AN1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -36787,7 +36802,7 @@
     <col min="21" max="39" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="90.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:40" ht="90.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -36905,8 +36920,11 @@
       <c r="AM1" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AN1" s="62" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31" t="s">
         <v>241</v>
       </c>
@@ -36962,7 +36980,7 @@
         <v>50311.8</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32" t="s">
         <v>245</v>
       </c>
@@ -37016,7 +37034,7 @@
         <v>50529.599999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
         <v>240</v>
       </c>
@@ -37072,7 +37090,7 @@
         <v>50856.3</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="32"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -37090,7 +37108,7 @@
       <c r="P5" s="34"/>
       <c r="AC5" s="34"/>
     </row>
-    <row r="6" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="31"/>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -37108,7 +37126,7 @@
       <c r="P6" s="33"/>
       <c r="AC6" s="33"/>
     </row>
-    <row r="7" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="32"/>
       <c r="B7" s="34"/>
       <c r="C7" s="34"/>
@@ -37126,7 +37144,7 @@
       <c r="P7" s="34"/>
       <c r="AC7" s="34"/>
     </row>
-    <row r="8" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="31"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -37144,7 +37162,7 @@
       <c r="P8" s="33"/>
       <c r="AC8" s="33"/>
     </row>
-    <row r="9" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -37162,7 +37180,7 @@
       <c r="P9" s="34"/>
       <c r="AC9" s="34"/>
     </row>
-    <row r="10" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="31"/>
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
@@ -37180,7 +37198,7 @@
       <c r="P10" s="33"/>
       <c r="AC10" s="33"/>
     </row>
-    <row r="11" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="32"/>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -37198,7 +37216,7 @@
       <c r="P11" s="34"/>
       <c r="AC11" s="34"/>
     </row>
-    <row r="12" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="31"/>
       <c r="B12" s="33"/>
       <c r="C12" s="33"/>
@@ -37216,7 +37234,7 @@
       <c r="P12" s="33"/>
       <c r="AC12" s="33"/>
     </row>
-    <row r="13" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="32"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
@@ -37234,7 +37252,7 @@
       <c r="P13" s="34"/>
       <c r="AC13" s="34"/>
     </row>
-    <row r="14" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="31"/>
       <c r="B14" s="33"/>
       <c r="C14" s="33"/>
@@ -37252,7 +37270,7 @@
       <c r="P14" s="33"/>
       <c r="AC14" s="33"/>
     </row>
-    <row r="15" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32"/>
       <c r="B15" s="34"/>
       <c r="C15" s="34"/>
@@ -37270,7 +37288,7 @@
       <c r="P15" s="34"/>
       <c r="AC15" s="34"/>
     </row>
-    <row r="16" spans="1:39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="31"/>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
@@ -39283,10 +39301,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AE988"/>
+  <dimension ref="A1:AF988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -39313,7 +39331,7 @@
     <col min="22" max="31" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:32" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -39407,8 +39425,11 @@
       <c r="AE1" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AF1" s="62" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="53" t="s">
         <v>248</v>
       </c>
@@ -39457,7 +39478,7 @@
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F3" s="13"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -39469,7 +39490,7 @@
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
     </row>
-    <row r="4" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -39480,7 +39501,7 @@
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
     </row>
-    <row r="5" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -39491,77 +39512,77 @@
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
     </row>
-    <row r="6" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N6" s="5"/>
       <c r="P6" s="5"/>
       <c r="R6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
     </row>
-    <row r="7" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N7" s="5"/>
       <c r="P7" s="5"/>
       <c r="R7" s="5"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
     </row>
-    <row r="8" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N8" s="5"/>
       <c r="P8" s="5"/>
       <c r="R8" s="5"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
     </row>
-    <row r="9" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N9" s="5"/>
       <c r="P9" s="5"/>
       <c r="R9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
     </row>
-    <row r="10" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N10" s="5"/>
       <c r="P10" s="5"/>
       <c r="R10" s="5"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
     </row>
-    <row r="11" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N11" s="5"/>
       <c r="P11" s="5"/>
       <c r="R11" s="5"/>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
     </row>
-    <row r="12" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N12" s="5"/>
       <c r="P12" s="5"/>
       <c r="R12" s="5"/>
       <c r="T12" s="5"/>
       <c r="U12" s="5"/>
     </row>
-    <row r="13" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N13" s="5"/>
       <c r="P13" s="5"/>
       <c r="R13" s="5"/>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
     </row>
-    <row r="14" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N14" s="5"/>
       <c r="P14" s="5"/>
       <c r="R14" s="5"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
     </row>
-    <row r="15" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N15" s="5"/>
       <c r="P15" s="5"/>
       <c r="R15" s="5"/>
       <c r="T15" s="5"/>
       <c r="U15" s="5"/>
     </row>
-    <row r="16" spans="1:31" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="N16" s="5"/>
       <c r="P16" s="5"/>
       <c r="R16" s="5"/>
@@ -46380,10 +46401,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AB997"/>
+  <dimension ref="A1:AC997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -46409,7 +46430,7 @@
     <col min="21" max="28" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="126" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" ht="126" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -46494,8 +46515,11 @@
       <c r="AB1" s="10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AC1" s="62" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="46" t="s">
         <v>243</v>
       </c>
@@ -46537,7 +46561,7 @@
       </c>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="47" t="s">
         <v>244</v>
       </c>
@@ -46577,7 +46601,7 @@
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="46" t="s">
         <v>246</v>
       </c>
@@ -46620,84 +46644,84 @@
         <v>4823852.3849999998</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K5" s="5"/>
       <c r="M5" s="5"/>
       <c r="O5" s="5"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K6" s="5"/>
       <c r="M6" s="5"/>
       <c r="O6" s="5"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
     </row>
-    <row r="7" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K7" s="5"/>
       <c r="M7" s="5"/>
       <c r="O7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
     </row>
-    <row r="8" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K8" s="5"/>
       <c r="M8" s="5"/>
       <c r="O8" s="5"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K9" s="5"/>
       <c r="M9" s="5"/>
       <c r="O9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
     </row>
-    <row r="10" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K10" s="5"/>
       <c r="M10" s="52"/>
       <c r="O10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K11" s="5"/>
       <c r="M11" s="5"/>
       <c r="O11" s="5"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K12" s="5"/>
       <c r="M12" s="5"/>
       <c r="O12" s="5"/>
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
     </row>
-    <row r="13" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K13" s="5"/>
       <c r="M13" s="5"/>
       <c r="O13" s="5"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
     </row>
-    <row r="14" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K14" s="5"/>
       <c r="M14" s="5"/>
       <c r="O14" s="5"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
     </row>
-    <row r="15" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K15" s="5"/>
       <c r="M15" s="5"/>
       <c r="O15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
     </row>
-    <row r="16" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="K16" s="5"/>
       <c r="M16" s="5"/>
       <c r="O16" s="5"/>

</xml_diff>

<commit_message>
validations for 50K, other categories, update spreadsheets
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/data-contracts/EOHHS-075-06302020-bad_proj_id-v1.xlsx
+++ b/tests/server/fixtures/data-contracts/EOHHS-075-06302020-bad_proj_id-v1.xlsx
@@ -18,17 +18,17 @@
     <sheet state="visible" name="Summary" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames>
+    <definedName name="Award">Dropdowns!$J$3:$J$4</definedName>
+    <definedName name="Compliance">Dropdowns!$K$3:$K$4</definedName>
+    <definedName name="Contracts">Dropdowns!$G$3:$G$6</definedName>
+    <definedName name="Agency">Dropdowns!$B$4:$B$27</definedName>
+    <definedName name="Country">Dropdowns!$F$3:$F$5</definedName>
+    <definedName name="UpdatesAI">Dropdowns!$P$3:$P$4</definedName>
+    <definedName name="OrganizationType">Dropdowns!$D$3:$D$22</definedName>
+    <definedName name="Organization">#REF!</definedName>
+    <definedName name="Status">Dropdowns!$C$3:$C$6</definedName>
+    <definedName name="State">Dropdowns!$E$3:$E$61</definedName>
     <definedName name="UpdatesAA">Dropdowns!$O$3:$O$4</definedName>
-    <definedName name="Organization">#REF!</definedName>
-    <definedName name="Country">Dropdowns!$F$3:$F$5</definedName>
-    <definedName name="Compliance">Dropdowns!$K$3:$K$4</definedName>
-    <definedName name="Agency">Dropdowns!$B$4:$B$27</definedName>
-    <definedName name="Status">Dropdowns!$C$3:$C$6</definedName>
-    <definedName name="UpdatesAI">Dropdowns!$P$3:$P$4</definedName>
-    <definedName name="Contracts">Dropdowns!$G$3:$G$6</definedName>
-    <definedName name="OrganizationType">Dropdowns!$D$3:$D$22</definedName>
-    <definedName name="Award">Dropdowns!$J$3:$J$4</definedName>
-    <definedName name="State">Dropdowns!$E$3:$E$61</definedName>
     <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">Contracts!$A$1:$AY$1</definedName>
   </definedNames>
   <calcPr/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="346">
   <si>
     <t>Certification</t>
   </si>
@@ -544,6 +544,9 @@
     <t>3673893</t>
   </si>
   <si>
+    <t>Other</t>
+  </si>
+  <si>
     <t>3674861</t>
   </si>
   <si>
@@ -899,9 +902,6 @@
   </si>
   <si>
     <t>ME</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>MH</t>
@@ -1316,7 +1316,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1368,11 +1368,23 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="8" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="3" fillId="8" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="8" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="8" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1805,9 +1817,6 @@
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="2"/>
@@ -1833,9 +1842,6 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="2"/>
@@ -1861,9 +1867,6 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="2"/>
@@ -1889,9 +1892,6 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="2"/>
@@ -1917,9 +1917,6 @@
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="2"/>
@@ -8499,6 +8496,10 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -8526,70 +8527,70 @@
   <sheetData>
     <row r="1" ht="37.5" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>140</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" s="16"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B3" s="16">
         <v>75.0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D3" s="42">
+        <v>217</v>
+      </c>
+      <c r="D3" s="46">
         <v>2163121.97</v>
       </c>
-      <c r="E3" s="42">
+      <c r="E3" s="46">
         <v>840542.45</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B4" s="16">
         <v>75.0</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D4" s="42">
+        <v>182</v>
+      </c>
+      <c r="D4" s="46">
         <v>5957909.0</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="46">
         <v>5957909.0</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B5" s="16"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B6" s="16"/>
     </row>
@@ -9616,26 +9617,26 @@
         <v>7</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>140</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="30">
+      <c r="A2" s="34">
         <v>75.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" s="37">
+        <v>182</v>
+      </c>
+      <c r="C2" s="41">
         <v>1567999.5</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="41">
         <v>1567999.5</v>
       </c>
     </row>
@@ -10662,120 +10663,120 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="43" t="s">
+      <c r="A1" s="47" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="B1" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="C1" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="43" t="s">
-        <v>224</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>214</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>224</v>
-      </c>
-      <c r="H1" s="43" t="s">
+      <c r="D1" s="47" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="E1" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="F1" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="43" t="s">
-        <v>215</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>217</v>
-      </c>
-      <c r="L1" s="43" t="s">
+      <c r="G1" s="47" t="s">
+        <v>225</v>
+      </c>
+      <c r="H1" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="M1" s="43" t="s">
-        <v>226</v>
-      </c>
-      <c r="N1" s="43" t="s">
+      <c r="I1" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>218</v>
+      </c>
+      <c r="L1" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
+      <c r="M1" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="N1" s="47" t="s">
+        <v>228</v>
+      </c>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="43" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>229</v>
-      </c>
-      <c r="F2" s="44" t="s">
+      <c r="E2" s="48" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="H2" s="44" t="s">
+      <c r="G2" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="I2" s="44" t="s">
-        <v>170</v>
-      </c>
-      <c r="J2" s="44" t="s">
+      <c r="H2" s="48" t="s">
         <v>232</v>
       </c>
-      <c r="K2" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="L2" s="44" t="s">
-        <v>211</v>
-      </c>
-      <c r="M2" s="44" t="s">
+      <c r="I2" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="L2" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="N2" s="44" t="s">
-        <v>212</v>
-      </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
+      <c r="M2" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="N2" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="43" t="s">
-        <v>233</v>
+      <c r="A3" s="47" t="s">
+        <v>234</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>12</v>
@@ -10784,140 +10785,140 @@
         <v>55</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G3" s="16">
         <v>1.0</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
       <c r="B4" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G4" s="16">
         <v>2.0</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="K4" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="M4" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="L4" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="M4" s="16" t="s">
-        <v>244</v>
-      </c>
       <c r="N4" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="1">
       <c r="B5" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>68</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="G5" s="45" t="s">
         <v>250</v>
       </c>
+      <c r="G5" s="49" t="s">
+        <v>251</v>
+      </c>
       <c r="L5" s="16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
       <c r="B6" s="16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
       <c r="C7" s="16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="C8" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="46" t="s">
-        <v>258</v>
+      <c r="E8" s="50" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="9" ht="15.0" customHeight="1">
@@ -10925,7 +10926,7 @@
         <v>93</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
@@ -10933,7 +10934,7 @@
         <v>98</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" ht="15.0" customHeight="1">
@@ -10941,15 +10942,15 @@
         <v>104</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="C12" s="17" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" ht="15.0" customHeight="1">
@@ -10957,7 +10958,7 @@
         <v>115</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" ht="15.0" customHeight="1">
@@ -10965,44 +10966,44 @@
         <v>121</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" ht="15.0" customHeight="1">
       <c r="C15" s="16" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="C16" s="16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" ht="15.0" customHeight="1">
       <c r="C17" s="16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="C18" s="16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" ht="15.0" customHeight="1">
       <c r="C19" s="16" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>79</v>
@@ -11010,55 +11011,55 @@
     </row>
     <row r="20" ht="15.0" customHeight="1">
       <c r="C20" s="16" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="C21" s="16" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="C22" s="17" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" ht="15.0" customHeight="1">
       <c r="C23" s="17" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" ht="15.0" customHeight="1">
       <c r="C24" s="17" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" ht="15.0" customHeight="1">
       <c r="C25" s="16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" ht="15.0" customHeight="1">
       <c r="C26" s="16" t="s">
-        <v>287</v>
+        <v>168</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>288</v>
@@ -12205,102 +12206,102 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="47" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="1">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="51" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="51" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="51" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="1">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="51" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="47" t="s">
         <v>327</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43" t="s">
+      <c r="E7" s="47"/>
+      <c r="F7" s="47" t="s">
         <v>328</v>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="43"/>
-      <c r="S7" s="43"/>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="43"/>
-      <c r="Z7" s="43"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+      <c r="X7" s="47"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="47"/>
     </row>
     <row r="8" ht="15.0" customHeight="1">
       <c r="A8" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="53"/>
     </row>
     <row r="9" ht="15.0" customHeight="1">
       <c r="A9" s="16" t="s">
         <v>330</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="49"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="53"/>
     </row>
     <row r="10" ht="15.0" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="48">
+      <c r="B10" s="53"/>
+      <c r="C10" s="52">
         <f>B8+B9</f>
         <v>0</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="48">
+      <c r="D10" s="53"/>
+      <c r="E10" s="52">
         <f>D8+D9</f>
         <v>0</v>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="48">
+      <c r="F10" s="53"/>
+      <c r="G10" s="52">
         <f>F8+F9</f>
         <v>0</v>
       </c>
@@ -12309,40 +12310,40 @@
       <c r="A11" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="49"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53"/>
     </row>
     <row r="12" ht="15.0" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="49"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53"/>
     </row>
     <row r="13" ht="15.0" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="48">
+      <c r="B13" s="53"/>
+      <c r="C13" s="52">
         <f>B11+B12</f>
         <v>0</v>
       </c>
-      <c r="D13" s="49"/>
-      <c r="E13" s="48">
+      <c r="D13" s="53"/>
+      <c r="E13" s="52">
         <f>D11+D12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="49"/>
-      <c r="G13" s="48">
+      <c r="F13" s="53"/>
+      <c r="G13" s="52">
         <f>F11+F12</f>
         <v>0</v>
       </c>
@@ -12351,40 +12352,40 @@
       <c r="A14" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="49"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" ht="15.0" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>336</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53"/>
     </row>
     <row r="16" ht="15.0" customHeight="1">
       <c r="A16" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="48">
+      <c r="B16" s="53"/>
+      <c r="C16" s="52">
         <f>B14+B15</f>
         <v>0</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="48">
+      <c r="D16" s="53"/>
+      <c r="E16" s="52">
         <f>D14+D15</f>
         <v>0</v>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="48">
+      <c r="F16" s="53"/>
+      <c r="G16" s="52">
         <f>F14+F15</f>
         <v>0</v>
       </c>
@@ -12393,40 +12394,40 @@
       <c r="A17" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="49"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="53"/>
     </row>
     <row r="18" ht="15.0" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="49"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" ht="15.0" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="48">
+      <c r="B19" s="53"/>
+      <c r="C19" s="52">
         <f>B17+B18</f>
         <v>0</v>
       </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="48">
+      <c r="D19" s="53"/>
+      <c r="E19" s="52">
         <f>D17+D18</f>
         <v>0</v>
       </c>
-      <c r="F19" s="49"/>
-      <c r="G19" s="48">
+      <c r="F19" s="53"/>
+      <c r="G19" s="52">
         <f>F17+F18</f>
         <v>0</v>
       </c>
@@ -12435,40 +12436,40 @@
       <c r="A20" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" ht="15.0" customHeight="1">
       <c r="A21" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="49"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53"/>
     </row>
     <row r="22" ht="15.0" customHeight="1">
       <c r="A22" s="16" t="s">
         <v>343</v>
       </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="48">
+      <c r="B22" s="53"/>
+      <c r="C22" s="52">
         <f>B20+B21</f>
         <v>0</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="48">
+      <c r="D22" s="53"/>
+      <c r="E22" s="52">
         <f>D20+D21</f>
         <v>0</v>
       </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="48">
+      <c r="F22" s="53"/>
+      <c r="G22" s="52">
         <f>F20+F21</f>
         <v>0</v>
       </c>
@@ -12477,51 +12478,51 @@
       <c r="A23" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="48"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="52"/>
     </row>
     <row r="24" ht="15.0" customHeight="1">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="47" t="s">
         <v>345</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50">
+      <c r="B24" s="54"/>
+      <c r="C24" s="54">
         <f>C10+C13+C16+C19+C22</f>
         <v>0</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50">
+      <c r="D24" s="54"/>
+      <c r="E24" s="54">
         <f>E10+E13+E16+E19+E22</f>
         <v>0</v>
       </c>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50">
+      <c r="F24" s="54"/>
+      <c r="G24" s="54">
         <f>G10+G13+G16+G19+G22</f>
         <v>0</v>
       </c>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="43"/>
-      <c r="T24" s="43"/>
-      <c r="U24" s="43"/>
-      <c r="V24" s="43"/>
-      <c r="W24" s="43"/>
-      <c r="X24" s="43"/>
-      <c r="Y24" s="43"/>
-      <c r="Z24" s="43"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="47"/>
+      <c r="V24" s="47"/>
+      <c r="W24" s="47"/>
+      <c r="X24" s="47"/>
+      <c r="Y24" s="47"/>
+      <c r="Z24" s="47"/>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>
@@ -20927,57 +20928,59 @@
         <v>44012.0</v>
       </c>
       <c r="V2" s="25">
-        <v>172.0</v>
-      </c>
-      <c r="W2" s="11"/>
+        <v>100172.0</v>
+      </c>
+      <c r="W2" s="26">
+        <v>100000.0</v>
+      </c>
       <c r="X2" s="11"/>
       <c r="Y2" s="11"/>
       <c r="Z2" s="11"/>
       <c r="AA2" s="11"/>
       <c r="AB2" s="11"/>
       <c r="AC2" s="11"/>
-      <c r="AD2" s="25">
+      <c r="AD2" s="27">
         <v>172.0</v>
       </c>
       <c r="AE2" s="11"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="28" t="s">
         <v>167</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="29">
         <v>537579.0</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="30">
         <v>43929.35916666667</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="30">
         <v>43929.35916666667</v>
       </c>
       <c r="H3" s="23">
         <v>44012.0</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="26"/>
+      <c r="J3" s="28"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="M3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="26" t="s">
+      <c r="N3" s="28" t="s">
         <v>80</v>
       </c>
       <c r="O3" s="11" t="s">
@@ -20989,30 +20992,35 @@
       <c r="R3" s="11">
         <v>75.0</v>
       </c>
-      <c r="S3" s="27">
+      <c r="S3" s="29">
         <v>537579.0</v>
       </c>
-      <c r="T3" s="28">
+      <c r="T3" s="30">
         <v>43929.35916666667</v>
       </c>
       <c r="U3" s="24">
         <v>44012.0</v>
       </c>
-      <c r="V3" s="29">
-        <v>19199.25</v>
-      </c>
-      <c r="W3" s="11"/>
+      <c r="V3" s="31">
+        <v>119199.25</v>
+      </c>
+      <c r="W3" s="26">
+        <v>100000.0</v>
+      </c>
       <c r="X3" s="11"/>
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
       <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
-      <c r="AD3" s="29">
+      <c r="AD3" s="32">
         <v>9199.25</v>
       </c>
       <c r="AE3" s="11"/>
-      <c r="AO3" s="30">
+      <c r="AN3" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="AO3" s="34">
         <v>10000.0</v>
       </c>
     </row>
@@ -21024,7 +21032,7 @@
         <v>106</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>165</v>
@@ -21074,16 +21082,18 @@
         <v>44012.0</v>
       </c>
       <c r="V4" s="25">
-        <v>13810.0</v>
-      </c>
-      <c r="W4" s="11"/>
+        <v>113810.0</v>
+      </c>
+      <c r="W4" s="26">
+        <v>100000.0</v>
+      </c>
       <c r="X4" s="11"/>
       <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
       <c r="AB4" s="11"/>
       <c r="AC4" s="11"/>
-      <c r="AD4" s="25">
+      <c r="AD4" s="27">
         <v>13810.0</v>
       </c>
       <c r="AE4" s="11"/>
@@ -23594,16 +23604,16 @@
         <v>123</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>128</v>
@@ -23612,13 +23622,13 @@
         <v>129</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>133</v>
@@ -23630,19 +23640,19 @@
         <v>135</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>137</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>139</v>
@@ -23721,14 +23731,14 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E2" s="21">
         <v>2927600.0</v>
@@ -23759,10 +23769,10 @@
       <c r="O2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="T2" s="30">
+      <c r="R2" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="T2" s="34">
         <v>75.0</v>
       </c>
       <c r="U2" s="21">
@@ -23772,13 +23782,13 @@
         <v>43969.64884259259</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="X2" s="25">
+        <v>183</v>
+      </c>
+      <c r="X2" s="27">
         <v>585520.0</v>
       </c>
       <c r="Y2" s="11"/>
-      <c r="Z2" s="25">
+      <c r="Z2" s="27">
         <v>585520.0</v>
       </c>
       <c r="AA2" s="11"/>
@@ -28337,22 +28347,22 @@
         <v>122</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>131</v>
@@ -28361,22 +28371,22 @@
         <v>132</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>135</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>137</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>140</v>
@@ -28385,13 +28395,13 @@
         <v>139</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="U1" s="18" t="s">
         <v>144</v>
@@ -28455,14 +28465,14 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="36" t="s">
         <v>69</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D2" s="20">
         <v>50311.8</v>
@@ -28494,85 +28504,85 @@
       <c r="M2" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="31" t="s">
-        <v>196</v>
+      <c r="O2" s="35" t="s">
+        <v>197</v>
       </c>
       <c r="P2" s="20">
         <v>50311.8</v>
       </c>
-      <c r="Q2" s="30">
+      <c r="Q2" s="34">
         <v>75.0</v>
       </c>
-      <c r="T2" s="30" t="s">
-        <v>181</v>
+      <c r="T2" s="34" t="s">
+        <v>182</v>
       </c>
       <c r="AC2" s="20">
         <v>50311.8</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" s="26">
+      <c r="C3" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="28">
         <v>50529.6</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="30">
         <v>43959.0</v>
       </c>
       <c r="F3" s="6">
         <v>44104.0</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26" t="s">
+      <c r="H3" s="28"/>
+      <c r="I3" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="28" t="s">
         <v>97</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="P3" s="26">
+      <c r="O3" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="P3" s="28">
         <v>50529.6</v>
       </c>
-      <c r="Q3" s="30">
+      <c r="Q3" s="34">
         <v>75.0</v>
       </c>
-      <c r="T3" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="AC3" s="26">
+      <c r="T3" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC3" s="28">
         <v>50529.6</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="36" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>64</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D4" s="20">
         <v>50856.3</v>
@@ -28604,42 +28614,42 @@
       <c r="M4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="31" t="s">
-        <v>196</v>
+      <c r="O4" s="35" t="s">
+        <v>197</v>
       </c>
       <c r="P4" s="20">
         <v>50856.3</v>
       </c>
-      <c r="Q4" s="30">
+      <c r="Q4" s="34">
         <v>75.0</v>
       </c>
-      <c r="T4" s="30" t="s">
-        <v>181</v>
+      <c r="T4" s="34" t="s">
+        <v>182</v>
       </c>
       <c r="AC4" s="20">
         <v>50856.3</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="33"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="28"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="26"/>
-      <c r="AC5" s="26"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="28"/>
+      <c r="AC5" s="28"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="32"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -28652,30 +28662,30 @@
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
-      <c r="O6" s="31"/>
+      <c r="O6" s="35"/>
       <c r="P6" s="20"/>
       <c r="AC6" s="20"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="33"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="28"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="O7" s="31"/>
-      <c r="P7" s="26"/>
-      <c r="AC7" s="26"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="O7" s="35"/>
+      <c r="P7" s="28"/>
+      <c r="AC7" s="28"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="32"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
@@ -28688,30 +28698,30 @@
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
-      <c r="O8" s="31"/>
+      <c r="O8" s="35"/>
       <c r="P8" s="20"/>
       <c r="AC8" s="20"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="28"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="30"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="26"/>
-      <c r="AC9" s="26"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="28"/>
+      <c r="AC9" s="28"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="32"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -28724,30 +28734,30 @@
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
       <c r="M10" s="20"/>
-      <c r="O10" s="31"/>
+      <c r="O10" s="35"/>
       <c r="P10" s="20"/>
       <c r="AC10" s="20"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="28"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="O11" s="31"/>
-      <c r="P11" s="26"/>
-      <c r="AC11" s="26"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="28"/>
+      <c r="AC11" s="28"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="32"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -28760,30 +28770,30 @@
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
-      <c r="O12" s="31"/>
+      <c r="O12" s="35"/>
       <c r="P12" s="20"/>
       <c r="AC12" s="20"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="28"/>
+      <c r="A13" s="37"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="26"/>
-      <c r="AC13" s="26"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="28"/>
+      <c r="AC13" s="28"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="32"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -28796,30 +28806,30 @@
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
       <c r="M14" s="20"/>
-      <c r="O14" s="31"/>
+      <c r="O14" s="35"/>
       <c r="P14" s="20"/>
       <c r="AC14" s="20"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="28"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="30"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="O15" s="31"/>
-      <c r="P15" s="26"/>
-      <c r="AC15" s="26"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="28"/>
+      <c r="AC15" s="28"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="32"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
@@ -28832,30 +28842,30 @@
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
-      <c r="O16" s="31"/>
+      <c r="O16" s="35"/>
       <c r="P16" s="20"/>
       <c r="AC16" s="20"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="33"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="28"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="26"/>
-      <c r="AC17" s="26"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="28"/>
+      <c r="AC17" s="28"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="32"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
@@ -28868,30 +28878,30 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
-      <c r="O18" s="31"/>
+      <c r="O18" s="35"/>
       <c r="P18" s="20"/>
       <c r="AC18" s="20"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="28"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="30"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="O19" s="31"/>
-      <c r="P19" s="26"/>
-      <c r="AC19" s="26"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="O19" s="35"/>
+      <c r="P19" s="28"/>
+      <c r="AC19" s="28"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="32"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
@@ -28904,30 +28914,30 @@
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
       <c r="M20" s="20"/>
-      <c r="O20" s="31"/>
+      <c r="O20" s="35"/>
       <c r="P20" s="20"/>
       <c r="AC20" s="20"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="33"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="28"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="30"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="26"/>
-      <c r="AC21" s="26"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="28"/>
+      <c r="AC21" s="28"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="32"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
@@ -28940,30 +28950,30 @@
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
-      <c r="O22" s="31"/>
+      <c r="O22" s="35"/>
       <c r="P22" s="20"/>
       <c r="AC22" s="20"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="33"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="28"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="26"/>
-      <c r="AC23" s="26"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="28"/>
+      <c r="AC23" s="28"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="32"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
@@ -28976,30 +28986,30 @@
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
-      <c r="O24" s="31"/>
+      <c r="O24" s="35"/>
       <c r="P24" s="20"/>
       <c r="AC24" s="20"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="33"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="28"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="30"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="26"/>
-      <c r="AC25" s="26"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="28"/>
+      <c r="AC25" s="28"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="32"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
@@ -29012,30 +29022,30 @@
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
       <c r="M26" s="20"/>
-      <c r="O26" s="31"/>
+      <c r="O26" s="35"/>
       <c r="P26" s="20"/>
       <c r="AC26" s="20"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="28"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="30"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="26"/>
-      <c r="AC27" s="26"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="28"/>
+      <c r="AC27" s="28"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="32"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
@@ -29048,30 +29058,30 @@
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
       <c r="M28" s="20"/>
-      <c r="O28" s="31"/>
+      <c r="O28" s="35"/>
       <c r="P28" s="20"/>
       <c r="AC28" s="20"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="33"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="28"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="30"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="26"/>
-      <c r="AC29" s="26"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="28"/>
+      <c r="AC29" s="28"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="32"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="20"/>
@@ -29084,30 +29094,30 @@
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
       <c r="M30" s="20"/>
-      <c r="O30" s="31"/>
+      <c r="O30" s="35"/>
       <c r="P30" s="20"/>
       <c r="AC30" s="20"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="33"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="28"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="30"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="26"/>
-      <c r="AC31" s="26"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="28"/>
+      <c r="AC31" s="28"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="32"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20"/>
       <c r="D32" s="20"/>
@@ -29120,30 +29130,30 @@
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
       <c r="M32" s="20"/>
-      <c r="O32" s="31"/>
+      <c r="O32" s="35"/>
       <c r="P32" s="20"/>
       <c r="AC32" s="20"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="33"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="28"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="30"/>
       <c r="F33" s="6"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="26"/>
-      <c r="AC33" s="26"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="28"/>
+      <c r="AC33" s="28"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="32"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
@@ -29156,30 +29166,30 @@
       <c r="K34" s="20"/>
       <c r="L34" s="20"/>
       <c r="M34" s="20"/>
-      <c r="O34" s="31"/>
+      <c r="O34" s="35"/>
       <c r="P34" s="20"/>
       <c r="AC34" s="20"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="33"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="28"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="30"/>
       <c r="F35" s="6"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="26"/>
-      <c r="AC35" s="26"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="28"/>
+      <c r="AC35" s="28"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="32"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
@@ -29192,30 +29202,30 @@
       <c r="K36" s="20"/>
       <c r="L36" s="20"/>
       <c r="M36" s="20"/>
-      <c r="O36" s="31"/>
+      <c r="O36" s="35"/>
       <c r="P36" s="20"/>
       <c r="AC36" s="20"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="33"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="28"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="30"/>
       <c r="F37" s="6"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
-      <c r="M37" s="26"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="26"/>
-      <c r="AC37" s="26"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="28"/>
+      <c r="AC37" s="28"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="32"/>
+      <c r="A38" s="36"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
@@ -29228,30 +29238,30 @@
       <c r="K38" s="20"/>
       <c r="L38" s="20"/>
       <c r="M38" s="20"/>
-      <c r="O38" s="31"/>
+      <c r="O38" s="35"/>
       <c r="P38" s="20"/>
       <c r="AC38" s="20"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="33"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="28"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="30"/>
       <c r="F39" s="6"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="26"/>
-      <c r="O39" s="31"/>
-      <c r="P39" s="26"/>
-      <c r="AC39" s="26"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="28"/>
+      <c r="AC39" s="28"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="32"/>
+      <c r="A40" s="36"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
@@ -29264,30 +29274,30 @@
       <c r="K40" s="20"/>
       <c r="L40" s="20"/>
       <c r="M40" s="20"/>
-      <c r="O40" s="31"/>
+      <c r="O40" s="35"/>
       <c r="P40" s="20"/>
       <c r="AC40" s="20"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="33"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="28"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="30"/>
       <c r="F41" s="6"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="26"/>
-      <c r="M41" s="26"/>
-      <c r="O41" s="31"/>
-      <c r="P41" s="26"/>
-      <c r="AC41" s="26"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="28"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="28"/>
+      <c r="AC41" s="28"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="32"/>
+      <c r="A42" s="36"/>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
       <c r="D42" s="20"/>
@@ -29300,30 +29310,30 @@
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
       <c r="M42" s="20"/>
-      <c r="O42" s="31"/>
+      <c r="O42" s="35"/>
       <c r="P42" s="20"/>
       <c r="AC42" s="20"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="33"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="28"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="30"/>
       <c r="F43" s="6"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="26"/>
-      <c r="K43" s="26"/>
-      <c r="L43" s="26"/>
-      <c r="M43" s="26"/>
-      <c r="O43" s="31"/>
-      <c r="P43" s="26"/>
-      <c r="AC43" s="26"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="28"/>
+      <c r="AC43" s="28"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="32"/>
+      <c r="A44" s="36"/>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
       <c r="D44" s="20"/>
@@ -29336,30 +29346,30 @@
       <c r="K44" s="20"/>
       <c r="L44" s="20"/>
       <c r="M44" s="20"/>
-      <c r="O44" s="31"/>
+      <c r="O44" s="35"/>
       <c r="P44" s="20"/>
       <c r="AC44" s="20"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="33"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="28"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="30"/>
       <c r="F45" s="6"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="26"/>
-      <c r="K45" s="26"/>
-      <c r="L45" s="26"/>
-      <c r="M45" s="26"/>
-      <c r="O45" s="31"/>
-      <c r="P45" s="26"/>
-      <c r="AC45" s="26"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="O45" s="35"/>
+      <c r="P45" s="28"/>
+      <c r="AC45" s="28"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="32"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
@@ -29372,30 +29382,30 @@
       <c r="K46" s="20"/>
       <c r="L46" s="20"/>
       <c r="M46" s="20"/>
-      <c r="O46" s="31"/>
+      <c r="O46" s="35"/>
       <c r="P46" s="20"/>
       <c r="AC46" s="20"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="33"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="28"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="30"/>
       <c r="F47" s="6"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="26"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="26"/>
-      <c r="AC47" s="26"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="28"/>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
+      <c r="O47" s="35"/>
+      <c r="P47" s="28"/>
+      <c r="AC47" s="28"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="32"/>
+      <c r="A48" s="36"/>
       <c r="B48" s="20"/>
       <c r="C48" s="20"/>
       <c r="D48" s="20"/>
@@ -29408,30 +29418,30 @@
       <c r="K48" s="20"/>
       <c r="L48" s="20"/>
       <c r="M48" s="20"/>
-      <c r="O48" s="31"/>
+      <c r="O48" s="35"/>
       <c r="P48" s="20"/>
       <c r="AC48" s="20"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="33"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="28"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="30"/>
       <c r="F49" s="6"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="O49" s="31"/>
-      <c r="P49" s="26"/>
-      <c r="AC49" s="26"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28"/>
+      <c r="O49" s="35"/>
+      <c r="P49" s="28"/>
+      <c r="AC49" s="28"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="32"/>
+      <c r="A50" s="36"/>
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
       <c r="D50" s="20"/>
@@ -29444,30 +29454,30 @@
       <c r="K50" s="20"/>
       <c r="L50" s="20"/>
       <c r="M50" s="20"/>
-      <c r="O50" s="31"/>
+      <c r="O50" s="35"/>
       <c r="P50" s="20"/>
       <c r="AC50" s="20"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="33"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="28"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="30"/>
       <c r="F51" s="6"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="26"/>
-      <c r="K51" s="26"/>
-      <c r="L51" s="26"/>
-      <c r="M51" s="26"/>
-      <c r="O51" s="31"/>
-      <c r="P51" s="26"/>
-      <c r="AC51" s="26"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="28"/>
+      <c r="K51" s="28"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="28"/>
+      <c r="O51" s="35"/>
+      <c r="P51" s="28"/>
+      <c r="AC51" s="28"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="32"/>
+      <c r="A52" s="36"/>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
@@ -29480,30 +29490,30 @@
       <c r="K52" s="20"/>
       <c r="L52" s="20"/>
       <c r="M52" s="20"/>
-      <c r="O52" s="31"/>
+      <c r="O52" s="35"/>
       <c r="P52" s="20"/>
       <c r="AC52" s="20"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="33"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="28"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="30"/>
       <c r="F53" s="6"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="26"/>
-      <c r="K53" s="26"/>
-      <c r="L53" s="26"/>
-      <c r="M53" s="26"/>
-      <c r="O53" s="31"/>
-      <c r="P53" s="26"/>
-      <c r="AC53" s="26"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="O53" s="35"/>
+      <c r="P53" s="28"/>
+      <c r="AC53" s="28"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="32"/>
+      <c r="A54" s="36"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
       <c r="D54" s="20"/>
@@ -29516,30 +29526,30 @@
       <c r="K54" s="20"/>
       <c r="L54" s="20"/>
       <c r="M54" s="20"/>
-      <c r="O54" s="31"/>
+      <c r="O54" s="35"/>
       <c r="P54" s="20"/>
       <c r="AC54" s="20"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="33"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="28"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="30"/>
       <c r="F55" s="6"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="26"/>
-      <c r="K55" s="26"/>
-      <c r="L55" s="26"/>
-      <c r="M55" s="26"/>
-      <c r="O55" s="31"/>
-      <c r="P55" s="26"/>
-      <c r="AC55" s="26"/>
+      <c r="G55" s="28"/>
+      <c r="H55" s="28"/>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="28"/>
+      <c r="O55" s="35"/>
+      <c r="P55" s="28"/>
+      <c r="AC55" s="28"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="32"/>
+      <c r="A56" s="36"/>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -29552,30 +29562,30 @@
       <c r="K56" s="20"/>
       <c r="L56" s="20"/>
       <c r="M56" s="20"/>
-      <c r="O56" s="31"/>
+      <c r="O56" s="35"/>
       <c r="P56" s="20"/>
       <c r="AC56" s="20"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="33"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="28"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="30"/>
       <c r="F57" s="6"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="26"/>
-      <c r="M57" s="26"/>
-      <c r="O57" s="31"/>
-      <c r="P57" s="26"/>
-      <c r="AC57" s="26"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="28"/>
+      <c r="O57" s="35"/>
+      <c r="P57" s="28"/>
+      <c r="AC57" s="28"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="32"/>
+      <c r="A58" s="36"/>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
       <c r="D58" s="20"/>
@@ -29588,30 +29598,30 @@
       <c r="K58" s="20"/>
       <c r="L58" s="20"/>
       <c r="M58" s="20"/>
-      <c r="O58" s="31"/>
+      <c r="O58" s="35"/>
       <c r="P58" s="20"/>
       <c r="AC58" s="20"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="33"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="28"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="30"/>
       <c r="F59" s="6"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
-      <c r="I59" s="26"/>
-      <c r="J59" s="26"/>
-      <c r="K59" s="26"/>
-      <c r="L59" s="26"/>
-      <c r="M59" s="26"/>
-      <c r="O59" s="31"/>
-      <c r="P59" s="26"/>
-      <c r="AC59" s="26"/>
+      <c r="G59" s="28"/>
+      <c r="H59" s="28"/>
+      <c r="I59" s="28"/>
+      <c r="J59" s="28"/>
+      <c r="K59" s="28"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="28"/>
+      <c r="O59" s="35"/>
+      <c r="P59" s="28"/>
+      <c r="AC59" s="28"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="32"/>
+      <c r="A60" s="36"/>
       <c r="B60" s="20"/>
       <c r="C60" s="20"/>
       <c r="D60" s="20"/>
@@ -29624,30 +29634,30 @@
       <c r="K60" s="20"/>
       <c r="L60" s="20"/>
       <c r="M60" s="20"/>
-      <c r="O60" s="31"/>
+      <c r="O60" s="35"/>
       <c r="P60" s="20"/>
       <c r="AC60" s="20"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="33"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="26"/>
-      <c r="E61" s="28"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="30"/>
       <c r="F61" s="6"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="26"/>
-      <c r="M61" s="26"/>
-      <c r="O61" s="31"/>
-      <c r="P61" s="26"/>
-      <c r="AC61" s="26"/>
+      <c r="G61" s="28"/>
+      <c r="H61" s="28"/>
+      <c r="I61" s="28"/>
+      <c r="J61" s="28"/>
+      <c r="K61" s="28"/>
+      <c r="L61" s="28"/>
+      <c r="M61" s="28"/>
+      <c r="O61" s="35"/>
+      <c r="P61" s="28"/>
+      <c r="AC61" s="28"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="32"/>
+      <c r="A62" s="36"/>
       <c r="B62" s="20"/>
       <c r="C62" s="20"/>
       <c r="D62" s="20"/>
@@ -29660,30 +29670,30 @@
       <c r="K62" s="20"/>
       <c r="L62" s="20"/>
       <c r="M62" s="20"/>
-      <c r="O62" s="31"/>
+      <c r="O62" s="35"/>
       <c r="P62" s="20"/>
       <c r="AC62" s="20"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="33"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="26"/>
-      <c r="E63" s="28"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="30"/>
       <c r="F63" s="6"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
-      <c r="I63" s="26"/>
-      <c r="J63" s="26"/>
-      <c r="K63" s="26"/>
-      <c r="L63" s="26"/>
-      <c r="M63" s="26"/>
-      <c r="O63" s="31"/>
-      <c r="P63" s="26"/>
-      <c r="AC63" s="26"/>
+      <c r="G63" s="28"/>
+      <c r="H63" s="28"/>
+      <c r="I63" s="28"/>
+      <c r="J63" s="28"/>
+      <c r="K63" s="28"/>
+      <c r="L63" s="28"/>
+      <c r="M63" s="28"/>
+      <c r="O63" s="35"/>
+      <c r="P63" s="28"/>
+      <c r="AC63" s="28"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="32"/>
+      <c r="A64" s="36"/>
       <c r="B64" s="20"/>
       <c r="C64" s="20"/>
       <c r="D64" s="20"/>
@@ -29696,30 +29706,30 @@
       <c r="K64" s="20"/>
       <c r="L64" s="20"/>
       <c r="M64" s="20"/>
-      <c r="O64" s="31"/>
+      <c r="O64" s="35"/>
       <c r="P64" s="20"/>
       <c r="AC64" s="20"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="33"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="26"/>
-      <c r="E65" s="28"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="30"/>
       <c r="F65" s="6"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
-      <c r="I65" s="26"/>
-      <c r="J65" s="26"/>
-      <c r="K65" s="26"/>
-      <c r="L65" s="26"/>
-      <c r="M65" s="26"/>
-      <c r="O65" s="31"/>
-      <c r="P65" s="26"/>
-      <c r="AC65" s="26"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="28"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="28"/>
+      <c r="O65" s="35"/>
+      <c r="P65" s="28"/>
+      <c r="AC65" s="28"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
-      <c r="A66" s="32"/>
+      <c r="A66" s="36"/>
       <c r="B66" s="20"/>
       <c r="C66" s="20"/>
       <c r="D66" s="20"/>
@@ -29732,30 +29742,30 @@
       <c r="K66" s="20"/>
       <c r="L66" s="20"/>
       <c r="M66" s="20"/>
-      <c r="O66" s="31"/>
+      <c r="O66" s="35"/>
       <c r="P66" s="20"/>
       <c r="AC66" s="20"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
-      <c r="A67" s="33"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="26"/>
-      <c r="E67" s="28"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="30"/>
       <c r="F67" s="6"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="26"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="26"/>
-      <c r="K67" s="26"/>
-      <c r="L67" s="26"/>
-      <c r="M67" s="26"/>
-      <c r="O67" s="31"/>
-      <c r="P67" s="26"/>
-      <c r="AC67" s="26"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="28"/>
+      <c r="K67" s="28"/>
+      <c r="L67" s="28"/>
+      <c r="M67" s="28"/>
+      <c r="O67" s="35"/>
+      <c r="P67" s="28"/>
+      <c r="AC67" s="28"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="32"/>
+      <c r="A68" s="36"/>
       <c r="B68" s="20"/>
       <c r="C68" s="20"/>
       <c r="D68" s="20"/>
@@ -29768,30 +29778,30 @@
       <c r="K68" s="20"/>
       <c r="L68" s="20"/>
       <c r="M68" s="20"/>
-      <c r="O68" s="31"/>
+      <c r="O68" s="35"/>
       <c r="P68" s="20"/>
       <c r="AC68" s="20"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
-      <c r="A69" s="33"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="26"/>
-      <c r="D69" s="26"/>
-      <c r="E69" s="28"/>
+      <c r="A69" s="37"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="30"/>
       <c r="F69" s="6"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="26"/>
-      <c r="I69" s="26"/>
-      <c r="J69" s="26"/>
-      <c r="K69" s="26"/>
-      <c r="L69" s="26"/>
-      <c r="M69" s="26"/>
-      <c r="O69" s="31"/>
-      <c r="P69" s="26"/>
-      <c r="AC69" s="26"/>
+      <c r="G69" s="28"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="28"/>
+      <c r="K69" s="28"/>
+      <c r="L69" s="28"/>
+      <c r="M69" s="28"/>
+      <c r="O69" s="35"/>
+      <c r="P69" s="28"/>
+      <c r="AC69" s="28"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
-      <c r="A70" s="32"/>
+      <c r="A70" s="36"/>
       <c r="B70" s="20"/>
       <c r="C70" s="20"/>
       <c r="D70" s="20"/>
@@ -29804,30 +29814,30 @@
       <c r="K70" s="20"/>
       <c r="L70" s="20"/>
       <c r="M70" s="20"/>
-      <c r="O70" s="31"/>
+      <c r="O70" s="35"/>
       <c r="P70" s="20"/>
       <c r="AC70" s="20"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
-      <c r="A71" s="33"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="26"/>
-      <c r="E71" s="28"/>
+      <c r="A71" s="37"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="30"/>
       <c r="F71" s="6"/>
-      <c r="G71" s="26"/>
-      <c r="H71" s="26"/>
-      <c r="I71" s="26"/>
-      <c r="J71" s="26"/>
-      <c r="K71" s="26"/>
-      <c r="L71" s="26"/>
-      <c r="M71" s="26"/>
-      <c r="O71" s="31"/>
-      <c r="P71" s="26"/>
-      <c r="AC71" s="26"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
+      <c r="K71" s="28"/>
+      <c r="L71" s="28"/>
+      <c r="M71" s="28"/>
+      <c r="O71" s="35"/>
+      <c r="P71" s="28"/>
+      <c r="AC71" s="28"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="32"/>
+      <c r="A72" s="36"/>
       <c r="B72" s="20"/>
       <c r="C72" s="20"/>
       <c r="D72" s="20"/>
@@ -29840,30 +29850,30 @@
       <c r="K72" s="20"/>
       <c r="L72" s="20"/>
       <c r="M72" s="20"/>
-      <c r="O72" s="31"/>
+      <c r="O72" s="35"/>
       <c r="P72" s="20"/>
       <c r="AC72" s="20"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
-      <c r="A73" s="33"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="26"/>
-      <c r="E73" s="28"/>
+      <c r="A73" s="37"/>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="30"/>
       <c r="F73" s="6"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="26"/>
-      <c r="I73" s="26"/>
-      <c r="J73" s="26"/>
-      <c r="K73" s="26"/>
-      <c r="L73" s="26"/>
-      <c r="M73" s="26"/>
-      <c r="O73" s="31"/>
-      <c r="P73" s="26"/>
-      <c r="AC73" s="26"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="28"/>
+      <c r="K73" s="28"/>
+      <c r="L73" s="28"/>
+      <c r="M73" s="28"/>
+      <c r="O73" s="35"/>
+      <c r="P73" s="28"/>
+      <c r="AC73" s="28"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="32"/>
+      <c r="A74" s="36"/>
       <c r="B74" s="20"/>
       <c r="C74" s="20"/>
       <c r="D74" s="20"/>
@@ -29876,27 +29886,27 @@
       <c r="K74" s="20"/>
       <c r="L74" s="20"/>
       <c r="M74" s="20"/>
-      <c r="O74" s="31"/>
+      <c r="O74" s="35"/>
       <c r="P74" s="20"/>
       <c r="AC74" s="20"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="33"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="28"/>
+      <c r="A75" s="37"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="30"/>
       <c r="F75" s="6"/>
-      <c r="G75" s="26"/>
-      <c r="H75" s="26"/>
-      <c r="I75" s="26"/>
-      <c r="J75" s="26"/>
-      <c r="K75" s="26"/>
-      <c r="L75" s="26"/>
-      <c r="M75" s="26"/>
-      <c r="O75" s="31"/>
-      <c r="P75" s="26"/>
-      <c r="AC75" s="26"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
+      <c r="I75" s="28"/>
+      <c r="J75" s="28"/>
+      <c r="K75" s="28"/>
+      <c r="L75" s="28"/>
+      <c r="M75" s="28"/>
+      <c r="O75" s="35"/>
+      <c r="P75" s="28"/>
+      <c r="AC75" s="28"/>
     </row>
     <row r="76" ht="12.75" customHeight="1"/>
     <row r="77" ht="12.75" customHeight="1"/>
@@ -30868,22 +30878,22 @@
         <v>122</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>139</v>
@@ -30962,31 +30972,31 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>111</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="25">
+        <v>206</v>
+      </c>
+      <c r="D2" s="27">
         <v>32416.32</v>
       </c>
       <c r="E2" s="22">
         <v>43987.643125</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="H2" s="30">
+        <v>208</v>
+      </c>
+      <c r="H2" s="34">
         <v>75.0</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="27">
         <v>32416.32</v>
       </c>
       <c r="J2" s="6">
@@ -30995,10 +31005,10 @@
       <c r="K2" s="6">
         <v>44012.0</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="27">
         <v>32416.32</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="27">
         <v>32416.32</v>
       </c>
       <c r="N2" s="11"/>
@@ -33373,13 +33383,13 @@
         <v>122</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>139</v>
@@ -33458,22 +33468,22 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="39">
         <v>2.101184477E7</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="40">
         <v>44008.0</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="34">
         <v>75.0</v>
       </c>
-      <c r="F2" s="35">
+      <c r="F2" s="39">
         <v>2.101184477E7</v>
       </c>
       <c r="G2" s="6">
@@ -33482,12 +33492,12 @@
       <c r="H2" s="6">
         <v>44012.0</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="39">
         <v>2.101184477E7</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
-      <c r="L2" s="37">
+      <c r="L2" s="41">
         <v>1.0505922385E7</v>
       </c>
       <c r="M2" s="11"/>
@@ -33500,22 +33510,22 @@
       <c r="R2" s="11"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="43">
         <v>1.578213759E7</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="44">
         <v>44008.0</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="34">
         <v>75.0</v>
       </c>
-      <c r="F3" s="39">
+      <c r="F3" s="43">
         <v>1.578213759E7</v>
       </c>
       <c r="G3" s="6">
@@ -33524,12 +33534,12 @@
       <c r="H3" s="6">
         <v>44012.0</v>
       </c>
-      <c r="I3" s="39">
+      <c r="I3" s="43">
         <v>1.578213759E7</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="37">
+      <c r="L3" s="41">
         <v>1.578213759E7</v>
       </c>
       <c r="M3" s="11"/>
@@ -33540,22 +33550,22 @@
       <c r="R3" s="11"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="39">
         <v>9647704.77</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="40">
         <v>44008.0</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="34">
         <v>75.0</v>
       </c>
-      <c r="F4" s="35">
+      <c r="F4" s="39">
         <v>9647704.77</v>
       </c>
       <c r="G4" s="6">
@@ -33564,12 +33574,12 @@
       <c r="H4" s="6">
         <v>44012.0</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="39">
         <v>9647704.77</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
-      <c r="L4" s="37">
+      <c r="L4" s="41">
         <v>4823852.385</v>
       </c>
       <c r="M4" s="11"/>
@@ -33578,7 +33588,7 @@
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
-      <c r="T4" s="37">
+      <c r="T4" s="41">
         <v>4823852.385</v>
       </c>
     </row>
@@ -33619,7 +33629,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="K10" s="11"/>
-      <c r="M10" s="41"/>
+      <c r="M10" s="45"/>
       <c r="O10" s="11"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>

</xml_diff>